<commit_message>
Fixed conditional expression values not adding to dependencies.
</commit_message>
<xml_diff>
--- a/samples/output.xlsx
+++ b/samples/output.xlsx
@@ -14,61 +14,201 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment ref="H2" authorId="0">
+      <text>
+        <t>Changed to fix a wrong value. Had value of 
+Should have the data type of Integer but was a value of 1.1.</t>
+      </text>
+    </comment>
+    <comment ref="H3" authorId="0">
+      <text>
+        <t>Changed to fix a wrong value. Had value of 
+Should have the data type of Integer but was a value of 2.22.</t>
+      </text>
+    </comment>
+    <comment ref="G4" authorId="0">
+      <text>
+        <t>Changed to fix a wrong value. Had value of 0.0
+Should have the data type of Integer but was a value of 0.</t>
+      </text>
+    </comment>
+    <comment ref="H4" authorId="0">
+      <text>
+        <t>Changed to fix a wrong value. Had value of 
+Should have the data type of Integer but was a value of 0.0.</t>
+      </text>
+    </comment>
+    <comment ref="G5" authorId="0">
+      <text>
+        <t>Changed to fix a wrong value. Had value of 4.0
+Should have the data type of Integer but was a value of 0.</t>
+      </text>
+    </comment>
+    <comment ref="H5" authorId="0">
+      <text>
+        <t>Changed to fix a wrong value. Had value of 
+Should have the data type of Integer but was a value of 0.0.</t>
+      </text>
+    </comment>
+    <comment ref="D6" authorId="0">
+      <text>
+        <t>Should have the data type of Decimal(10,4) but was a value of 5.55555.</t>
+      </text>
+    </comment>
+    <comment ref="C6" authorId="0">
+      <text>
+        <t>This cell is required and should not be blank
+Should have the data type of Decimal(10,4) but was a value of .</t>
+      </text>
+    </comment>
+    <comment ref="A7" authorId="0">
+      <text>
+        <t>This cell is required and should not be blank
+Should have the data type of Integer but was a value of .</t>
+      </text>
+    </comment>
+    <comment ref="D7" authorId="0">
+      <text>
+        <t>Should have the data type of Decimal(10,4) but was a value of 6.666666.</t>
+      </text>
+    </comment>
+    <comment ref="B8" authorId="0">
+      <text>
+        <t>This cell is required and should not be blank
+Should have the data type of Integer but was a value of .</t>
+      </text>
+    </comment>
+    <comment ref="D8" authorId="0">
+      <text>
+        <t>Should have the data type of Decimal(10,4) but was a value of 7.7777777.</t>
+      </text>
+    </comment>
+    <comment ref="F8" authorId="0">
+      <text>
+        <t>Should have the data type of Enumerable "Enum1Val1" "Enum1Val2" "Enum1Val3" but was a value of aWrongVal.</t>
+      </text>
+    </comment>
+    <comment ref="D9" authorId="0">
+      <text>
+        <t>This cell is required and should not be blank
+Should have the data type of Decimal(10,4) but was a value of .</t>
+      </text>
+    </comment>
+    <comment ref="F9" authorId="0">
+      <text>
+        <t>Should have the data type of Enumerable "Enum1Val1" "Enum1Val2" "Enum1Val3" but was a value of another wrong.</t>
+      </text>
+    </comment>
+    <comment ref="D10" authorId="0">
+      <text>
+        <t>Should have the data type of Decimal(10,4) but was a value of 9.999999999.</t>
+      </text>
+    </comment>
+    <comment ref="F10" authorId="0">
+      <text>
+        <t>Should have the data type of Enumerable "Enum1Val1" "Enum1Val2" "Enum1Val3" but was a value of EnumVal11.</t>
+      </text>
+    </comment>
+    <comment ref="D11" authorId="0">
+      <text>
+        <t>Should have the data type of Decimal(10,4) but was a value of 10.101010101.</t>
+      </text>
+    </comment>
+    <comment ref="F11" authorId="0">
+      <text>
+        <t>This cell is required and should not be blank
+Should have the data type of Enumerable "Enum1Val1" "Enum1Val2" "Enum1Val3" but was a value of .</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
-  <si>
-    <t>SomeIntegers</t>
-  </si>
-  <si>
-    <t>SomeDecimals</t>
-  </si>
-  <si>
-    <t>SomeWords</t>
-  </si>
-  <si>
-    <t>SomeEnums</t>
-  </si>
-  <si>
-    <t>SomeInt&gt;5</t>
-  </si>
-  <si>
-    <t>SomeDec&lt;4</t>
-  </si>
-  <si>
-    <t>SomeEnumsIsValid</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
+  <si>
+    <t>InputInt1</t>
+  </si>
+  <si>
+    <t>InputInt2</t>
+  </si>
+  <si>
+    <t>InputDec1</t>
+  </si>
+  <si>
+    <t>InputDec2</t>
+  </si>
+  <si>
+    <t>InputStr1</t>
+  </si>
+  <si>
+    <t>InputEnum1</t>
+  </si>
+  <si>
+    <t>OutputInt1</t>
+  </si>
+  <si>
+    <t>OutputDec1</t>
   </si>
   <si>
     <t>Hello</t>
   </si>
   <si>
-    <t>enumVal1</t>
+    <t>Enum1Val1</t>
   </si>
   <si>
     <t>World</t>
   </si>
   <si>
-    <t>enumVal2</t>
+    <t>Enum1Val2</t>
   </si>
   <si>
     <t>foo</t>
   </si>
   <si>
-    <t>enumVal3</t>
+    <t>Enum1Val3</t>
   </si>
   <si>
     <t>bar</t>
   </si>
   <si>
-    <t>foobar</t>
-  </si>
-  <si>
-    <t>enumVal4</t>
-  </si>
-  <si>
-    <t>invalidValue</t>
-  </si>
-  <si>
-    <t>anotherInvalid</t>
+    <t>baz</t>
+  </si>
+  <si>
+    <t>fizz</t>
+  </si>
+  <si>
+    <t>buzz</t>
+  </si>
+  <si>
+    <t>aWrongVal</t>
+  </si>
+  <si>
+    <t>a string</t>
+  </si>
+  <si>
+    <t>another wrong</t>
+  </si>
+  <si>
+    <t>EnumVal11</t>
+  </si>
+  <si>
+    <t>1.1</t>
+  </si>
+  <si>
+    <t>2.22</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>0.0</t>
   </si>
 </sst>
 </file>
@@ -83,6 +223,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -100,12 +241,37 @@
       <family val="0"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="3"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="3"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="2"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -140,10 +306,137 @@
     <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="32">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -159,15 +452,19 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing"/>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -203,19 +500,34 @@
       <c r="G1" s="0" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C2" s="0" t="n">
         <v>1.1</v>
       </c>
-      <c r="C2" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="0" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="E2" s="0" t="s">
         <v>8</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H2" t="s" s="3">
+        <v>22</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -223,13 +535,25 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="D3" s="0" t="n">
         <v>2.22</v>
       </c>
-      <c r="C3" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="0" t="s">
+      <c r="E3" s="0" t="s">
         <v>10</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="H3" t="s" s="5">
+        <v>23</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -237,13 +561,25 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>3.3</v>
+      </c>
+      <c r="D4" s="0" t="n">
         <v>3.333</v>
       </c>
-      <c r="C4" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="0" t="s">
+      <c r="E4" s="0" t="s">
         <v>12</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" t="s" s="9">
+        <v>25</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -251,13 +587,25 @@
         <v>4</v>
       </c>
       <c r="B5" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>4.4</v>
+      </c>
+      <c r="D5" s="0" t="n">
         <v>4.4444</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="E5" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="0" t="s">
-        <v>12</v>
+      <c r="G5" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="H5" t="s" s="13">
+        <v>25</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -265,35 +613,62 @@
         <v>5</v>
       </c>
       <c r="B6" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="C6" s="16"/>
+      <c r="D6" s="14" t="n">
         <v>5.55555</v>
       </c>
-      <c r="C6" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>10</v>
+      <c r="E6" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="n">
-        <v>6</v>
-      </c>
+      <c r="A7" s="18"/>
       <c r="B7" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>6.6</v>
+      </c>
+      <c r="D7" s="19" t="n">
         <v>6.666666</v>
       </c>
-      <c r="D7" s="0" t="s">
-        <v>8</v>
+      <c r="E7" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" s="0" t="n">
+        <v>30</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="B8" s="0" t="n">
+      <c r="B8" s="21"/>
+      <c r="C8" s="0" t="n">
+        <v>7.7</v>
+      </c>
+      <c r="D8" s="22" t="n">
         <v>7.7777777</v>
       </c>
-      <c r="D8" s="0" t="s">
-        <v>15</v>
+      <c r="E8" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -301,10 +676,18 @@
         <v>8</v>
       </c>
       <c r="B9" s="0" t="n">
-        <v>8.88888888</v>
-      </c>
-      <c r="D9" s="0" t="s">
         <v>16</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>8.8</v>
+      </c>
+      <c r="D9" s="25"/>
+      <c r="F9" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" s="1" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -312,10 +695,16 @@
         <v>9</v>
       </c>
       <c r="B10" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>9.9</v>
+      </c>
+      <c r="D10" s="27" t="n">
         <v>9.999999999</v>
       </c>
-      <c r="D10" s="0" t="s">
-        <v>17</v>
+      <c r="F10" s="28" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -323,8 +712,15 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>10.1</v>
+      </c>
+      <c r="D11" s="29" t="n">
         <v>10.101010101</v>
       </c>
+      <c r="F11" s="31"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -334,5 +730,7 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Major overhaul to ExcelChecker to implement dependency digraph. Temporarily disabled auto-filling.
</commit_message>
<xml_diff>
--- a/samples/output.xlsx
+++ b/samples/output.xlsx
@@ -22,108 +22,237 @@
   <commentList>
     <comment ref="H2" authorId="0">
       <text>
-        <t>Changed to fix a wrong value. Had value of 
-Should have the data type of Integer but was a value of 1.1.</t>
+        <t>--- Format Errors
+This cell is required and should not be blank.
+Has the wrong value filled in.
+Should have the data type of Integer but was a value of "".</t>
       </text>
     </comment>
     <comment ref="H3" authorId="0">
       <text>
-        <t>Changed to fix a wrong value. Had value of 
-Should have the data type of Integer but was a value of 2.22.</t>
+        <t>--- Format Errors
+This cell is required and should not be blank.
+Has the wrong value filled in.
+Should have the data type of Integer but was a value of "".</t>
       </text>
     </comment>
     <comment ref="G4" authorId="0">
       <text>
-        <t>Changed to fix a wrong value. Had value of 0.0
-Should have the data type of Integer but was a value of 0.</t>
+        <t>--- Format Errors
+Has the wrong value filled in.</t>
       </text>
     </comment>
     <comment ref="H4" authorId="0">
       <text>
-        <t>Changed to fix a wrong value. Had value of 
-Should have the data type of Integer but was a value of 0.0.</t>
+        <t>--- Format Errors
+This cell is required and should not be blank.
+Has the wrong value filled in.
+Should have the data type of Integer but was a value of "".</t>
       </text>
     </comment>
     <comment ref="G5" authorId="0">
       <text>
-        <t>Changed to fix a wrong value. Had value of 4.0
-Should have the data type of Integer but was a value of 0.</t>
+        <t>--- Format Errors
+Has the wrong value filled in.</t>
       </text>
     </comment>
     <comment ref="H5" authorId="0">
       <text>
-        <t>Changed to fix a wrong value. Had value of 
-Should have the data type of Integer but was a value of 0.0.</t>
+        <t>--- Format Errors
+This cell is required and should not be blank.
+Has the wrong value filled in.
+Should have the data type of Integer but was a value of "".</t>
+      </text>
+    </comment>
+    <comment ref="G6" authorId="0">
+      <text>
+        <t>--- Format Errors
+Has the wrong value filled in.</t>
       </text>
     </comment>
     <comment ref="D6" authorId="0">
       <text>
-        <t>Should have the data type of Decimal(10,4) but was a value of 5.55555.</t>
+        <t>--- Format Errors
+Should have the data type of Decimal(10,4) but was a value of "5.55555".
+--- Critical Errors
+Cell OutputDec1 needs this cell to be nicely filled before it can be checked</t>
       </text>
     </comment>
     <comment ref="C6" authorId="0">
       <text>
-        <t>This cell is required and should not be blank
-Should have the data type of Decimal(10,4) but was a value of .</t>
+        <t>--- Format Errors
+This cell is required and should not be blank.
+Should have the data type of Decimal(10,4) but was a value of "".
+--- Critical Errors
+Cell OutputDec1 needs this cell to be nicely filled before it can be checked</t>
+      </text>
+    </comment>
+    <comment ref="H6" authorId="0">
+      <text>
+        <t>Could not check cell because it depends on poorly filled cells. This cell depended on cells InputDec2 and InputDec1</t>
       </text>
     </comment>
     <comment ref="A7" authorId="0">
       <text>
-        <t>This cell is required and should not be blank
-Should have the data type of Integer but was a value of .</t>
+        <t>--- Format Errors
+This cell is required and should not be blank.
+Should have the data type of Integer but was a value of "".
+--- Critical Errors
+Cell OutputInt1 needs this cell to be nicely filled before it can be checked</t>
+      </text>
+    </comment>
+    <comment ref="G7" authorId="0">
+      <text>
+        <t>Could not check cell because it depends on poorly filled cells. This cell depended on cells InputInt1</t>
       </text>
     </comment>
     <comment ref="D7" authorId="0">
       <text>
-        <t>Should have the data type of Decimal(10,4) but was a value of 6.666666.</t>
+        <t>--- Format Errors
+Should have the data type of Decimal(10,4) but was a value of "6.666666".
+--- Critical Errors
+Cell OutputDec1 needs this cell to be nicely filled before it can be checked</t>
+      </text>
+    </comment>
+    <comment ref="H7" authorId="0">
+      <text>
+        <t>Could not check cell because it depends on poorly filled cells. This cell depended on cells InputDec2</t>
       </text>
     </comment>
     <comment ref="B8" authorId="0">
       <text>
-        <t>This cell is required and should not be blank
-Should have the data type of Integer but was a value of .</t>
+        <t>--- Format Errors
+This cell is required and should not be blank.
+Should have the data type of Integer but was a value of "".
+--- Critical Errors
+Cell OutputInt1 needs this cell to be nicely filled before it can be checked</t>
+      </text>
+    </comment>
+    <comment ref="F8" authorId="0">
+      <text>
+        <t>--- Format Errors
+Should have the data type of Enumerable "Enum1Val1" "Enum1Val2" "Enum1Val3" but was a value of "aWrongVal".
+--- Critical Errors
+Cell OutputInt1 needs this cell to be nicely filled before it can be checked</t>
+      </text>
+    </comment>
+    <comment ref="G8" authorId="0">
+      <text>
+        <t>Could not check cell because it depends on poorly filled cells. This cell depended on cells InputInt2 and InputEnum1</t>
       </text>
     </comment>
     <comment ref="D8" authorId="0">
       <text>
-        <t>Should have the data type of Decimal(10,4) but was a value of 7.7777777.</t>
-      </text>
-    </comment>
-    <comment ref="F8" authorId="0">
-      <text>
-        <t>Should have the data type of Enumerable "Enum1Val1" "Enum1Val2" "Enum1Val3" but was a value of aWrongVal.</t>
+        <t>--- Format Errors
+Should have the data type of Decimal(10,4) but was a value of "7.7777777".
+--- Critical Errors
+Cell OutputDec1 needs this cell to be nicely filled before it can be checked</t>
+      </text>
+    </comment>
+    <comment ref="H8" authorId="0">
+      <text>
+        <t>Could not check cell because it depends on poorly filled cells. This cell depended on cells InputDec2</t>
+      </text>
+    </comment>
+    <comment ref="F9" authorId="0">
+      <text>
+        <t>--- Format Errors
+Should have the data type of Enumerable "Enum1Val1" "Enum1Val2" "Enum1Val3" but was a value of "another wrong".
+--- Critical Errors
+Cell OutputInt1 needs this cell to be nicely filled before it can be checked</t>
+      </text>
+    </comment>
+    <comment ref="G9" authorId="0">
+      <text>
+        <t>Could not check cell because it depends on poorly filled cells. This cell depended on cells InputEnum1</t>
       </text>
     </comment>
     <comment ref="D9" authorId="0">
       <text>
-        <t>This cell is required and should not be blank
-Should have the data type of Decimal(10,4) but was a value of .</t>
-      </text>
-    </comment>
-    <comment ref="F9" authorId="0">
-      <text>
-        <t>Should have the data type of Enumerable "Enum1Val1" "Enum1Val2" "Enum1Val3" but was a value of another wrong.</t>
+        <t>--- Format Errors
+This cell is required and should not be blank.
+Should have the data type of Decimal(10,4) but was a value of "".
+--- Critical Errors
+Cell OutputDec1 needs this cell to be nicely filled before it can be checked</t>
+      </text>
+    </comment>
+    <comment ref="H9" authorId="0">
+      <text>
+        <t>Could not check cell because it depends on poorly filled cells. This cell depended on cells InputDec2</t>
+      </text>
+    </comment>
+    <comment ref="E9" authorId="0">
+      <text>
+        <t>--- Format Errors
+This cell is required and should not be blank.
+Should have the data type of String but was a value of "".</t>
+      </text>
+    </comment>
+    <comment ref="F10" authorId="0">
+      <text>
+        <t>--- Format Errors
+Should have the data type of Enumerable "Enum1Val1" "Enum1Val2" "Enum1Val3" but was a value of "EnumVal11".
+--- Critical Errors
+Cell OutputInt1 needs this cell to be nicely filled before it can be checked</t>
+      </text>
+    </comment>
+    <comment ref="G10" authorId="0">
+      <text>
+        <t>Could not check cell because it depends on poorly filled cells. This cell depended on cells InputEnum1</t>
       </text>
     </comment>
     <comment ref="D10" authorId="0">
       <text>
-        <t>Should have the data type of Decimal(10,4) but was a value of 9.999999999.</t>
-      </text>
-    </comment>
-    <comment ref="F10" authorId="0">
-      <text>
-        <t>Should have the data type of Enumerable "Enum1Val1" "Enum1Val2" "Enum1Val3" but was a value of EnumVal11.</t>
+        <t>--- Format Errors
+Should have the data type of Decimal(10,4) but was a value of "9.999999999".
+--- Critical Errors
+Cell OutputDec1 needs this cell to be nicely filled before it can be checked</t>
+      </text>
+    </comment>
+    <comment ref="H10" authorId="0">
+      <text>
+        <t>Could not check cell because it depends on poorly filled cells. This cell depended on cells InputDec2</t>
+      </text>
+    </comment>
+    <comment ref="E10" authorId="0">
+      <text>
+        <t>--- Format Errors
+This cell is required and should not be blank.
+Should have the data type of String but was a value of "".</t>
+      </text>
+    </comment>
+    <comment ref="F11" authorId="0">
+      <text>
+        <t>--- Format Errors
+This cell is required and should not be blank.
+Should have the data type of Enumerable "Enum1Val1" "Enum1Val2" "Enum1Val3" but was a value of "".
+--- Critical Errors
+Cell OutputInt1 needs this cell to be nicely filled before it can be checked</t>
+      </text>
+    </comment>
+    <comment ref="G11" authorId="0">
+      <text>
+        <t>Could not check cell because it depends on poorly filled cells. This cell depended on cells InputEnum1</t>
       </text>
     </comment>
     <comment ref="D11" authorId="0">
       <text>
-        <t>Should have the data type of Decimal(10,4) but was a value of 10.101010101.</t>
-      </text>
-    </comment>
-    <comment ref="F11" authorId="0">
-      <text>
-        <t>This cell is required and should not be blank
-Should have the data type of Enumerable "Enum1Val1" "Enum1Val2" "Enum1Val3" but was a value of .</t>
+        <t>--- Format Errors
+Should have the data type of Decimal(10,4) but was a value of "10.101010101".
+--- Critical Errors
+Cell OutputDec1 needs this cell to be nicely filled before it can be checked</t>
+      </text>
+    </comment>
+    <comment ref="H11" authorId="0">
+      <text>
+        <t>Could not check cell because it depends on poorly filled cells. This cell depended on cells InputDec2</t>
+      </text>
+    </comment>
+    <comment ref="E11" authorId="0">
+      <text>
+        <t>--- Format Errors
+This cell is required and should not be blank.
+Should have the data type of String but was a value of "".</t>
       </text>
     </comment>
   </commentList>
@@ -131,7 +260,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
   <si>
     <t>InputInt1</t>
   </si>
@@ -197,18 +326,6 @@
   </si>
   <si>
     <t>EnumVal11</t>
-  </si>
-  <si>
-    <t>1.1</t>
-  </si>
-  <si>
-    <t>2.22</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>0.0</t>
   </si>
 </sst>
 </file>
@@ -241,7 +358,7 @@
       <family val="0"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -250,22 +367,12 @@
     </fill>
     <fill>
       <patternFill>
-        <fgColor indexed="3"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="3"/>
+        <fgColor indexed="5"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="5"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill>
-        <fgColor indexed="2"/>
       </patternFill>
     </fill>
     <fill>
@@ -311,7 +418,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="114">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -324,119 +431,447 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -526,9 +961,7 @@
       <c r="G2" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="H2" t="s" s="3">
-        <v>22</v>
-      </c>
+      <c r="H2" s="5"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
@@ -552,9 +985,7 @@
       <c r="G3" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="H3" t="s" s="5">
-        <v>23</v>
-      </c>
+      <c r="H3" s="9"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
@@ -575,12 +1006,10 @@
       <c r="F4" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="H4" t="s" s="9">
-        <v>25</v>
-      </c>
+      <c r="G4" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" s="15"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
@@ -601,12 +1030,10 @@
       <c r="F5" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="G5" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="H5" t="s" s="13">
-        <v>25</v>
-      </c>
+      <c r="G5" s="17" t="n">
+        <v>4</v>
+      </c>
+      <c r="H5" s="21"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
@@ -615,8 +1042,8 @@
       <c r="B6" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="C6" s="16"/>
-      <c r="D6" s="14" t="n">
+      <c r="C6" s="35"/>
+      <c r="D6" s="32" t="n">
         <v>5.55555</v>
       </c>
       <c r="E6" s="0" t="s">
@@ -625,19 +1052,20 @@
       <c r="F6" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="0" t="n">
+      <c r="G6" s="23" t="n">
         <v>20</v>
       </c>
+      <c r="H6" s="29"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="18"/>
+      <c r="A7" s="42"/>
       <c r="B7" s="0" t="n">
         <v>12</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>6.6</v>
       </c>
-      <c r="D7" s="19" t="n">
+      <c r="D7" s="48" t="n">
         <v>6.666666</v>
       </c>
       <c r="E7" s="0" t="s">
@@ -646,30 +1074,32 @@
       <c r="F7" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="G7" s="0" t="n">
+      <c r="G7" s="39" t="n">
         <v>30</v>
       </c>
+      <c r="H7" s="45"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="B8" s="21"/>
+      <c r="B8" s="57"/>
       <c r="C8" s="0" t="n">
         <v>7.7</v>
       </c>
-      <c r="D8" s="22" t="n">
+      <c r="D8" s="66" t="n">
         <v>7.7777777</v>
       </c>
       <c r="E8" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="F8" s="23" t="s">
+      <c r="F8" s="60" t="s">
         <v>18</v>
       </c>
-      <c r="G8" s="0" t="s">
+      <c r="G8" s="54" t="s">
         <v>19</v>
       </c>
+      <c r="H8" s="63"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
@@ -681,14 +1111,16 @@
       <c r="C9" s="0" t="n">
         <v>8.8</v>
       </c>
-      <c r="D9" s="25"/>
-      <c r="F9" s="26" t="s">
+      <c r="D9" s="79"/>
+      <c r="E9" s="82"/>
+      <c r="F9" s="72" t="s">
         <v>20</v>
       </c>
-      <c r="G9" s="1" t="n">
+      <c r="G9" s="69" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
+      <c r="H9" s="76"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
@@ -700,12 +1132,15 @@
       <c r="C10" s="0" t="n">
         <v>9.9</v>
       </c>
-      <c r="D10" s="27" t="n">
+      <c r="D10" s="94" t="n">
         <v>9.999999999</v>
       </c>
-      <c r="F10" s="28" t="s">
+      <c r="E10" s="97"/>
+      <c r="F10" s="88" t="s">
         <v>21</v>
       </c>
+      <c r="G10" s="85"/>
+      <c r="H10" s="91"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
@@ -717,10 +1152,13 @@
       <c r="C11" s="0" t="n">
         <v>10.1</v>
       </c>
-      <c r="D11" s="29" t="n">
+      <c r="D11" s="110" t="n">
         <v>10.101010101</v>
       </c>
-      <c r="F11" s="31"/>
+      <c r="E11" s="113"/>
+      <c r="F11" s="104"/>
+      <c r="G11" s="101"/>
+      <c r="H11" s="107"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Began reorganizing packages and fixing the GUI
</commit_message>
<xml_diff>
--- a/samples/output.xlsx
+++ b/samples/output.xlsx
@@ -20,6 +20,11 @@
     <author/>
   </authors>
   <commentList>
+    <comment ref="J2" authorId="0">
+      <text>
+        <t>Deleted content since not required. Value was Hello</t>
+      </text>
+    </comment>
     <comment ref="H2" authorId="0">
       <text>
         <t>Changed to fix a wrong value. Had value of "".</t>
@@ -30,6 +35,11 @@
         <t>Changed to fix a wrong value. Had value of "".</t>
       </text>
     </comment>
+    <comment ref="J3" authorId="0">
+      <text>
+        <t>Deleted content since not required. Value was 10.0</t>
+      </text>
+    </comment>
     <comment ref="H3" authorId="0">
       <text>
         <t>Changed to fix a wrong value. Had value of "".</t>
@@ -40,6 +50,11 @@
         <t>Changed to fix a wrong value. Had value of "".</t>
       </text>
     </comment>
+    <comment ref="J4" authorId="0">
+      <text>
+        <t>Deleted content since not required. Value was World</t>
+      </text>
+    </comment>
     <comment ref="H4" authorId="0">
       <text>
         <t>Changed to fix a wrong value. Had value of "".</t>
@@ -50,6 +65,11 @@
         <t>Changed to fix a wrong value. Had value of "".</t>
       </text>
     </comment>
+    <comment ref="J5" authorId="0">
+      <text>
+        <t>Deleted content since not required. Value was 10.222</t>
+      </text>
+    </comment>
     <comment ref="H5" authorId="0">
       <text>
         <t>Changed to fix a wrong value. Had value of "".</t>
@@ -58,6 +78,11 @@
     <comment ref="I5" authorId="0">
       <text>
         <t>Changed to fix a wrong value. Had value of "".</t>
+      </text>
+    </comment>
+    <comment ref="J6" authorId="0">
+      <text>
+        <t>Deleted content since not required. Value was EnumVal1</t>
       </text>
     </comment>
     <comment ref="C6" authorId="0">
@@ -296,7 +321,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="34">
   <si>
     <t>InputInt1</t>
   </si>
@@ -325,6 +350,9 @@
     <t>AutoFill1</t>
   </si>
   <si>
+    <t>NotRequired</t>
+  </si>
+  <si>
     <t>1.1</t>
   </si>
   <si>
@@ -352,6 +380,9 @@
     <t>baz</t>
   </si>
   <si>
+    <t>EnumVal1</t>
+  </si>
+  <si>
     <t>fizz</t>
   </si>
   <si>
@@ -364,7 +395,10 @@
     <t>EnumVal11</t>
   </si>
   <si>
-    <t>OK</t>
+    <t>lonely</t>
+  </si>
+  <si>
+    <t/>
   </si>
   <si>
     <t>Val1</t>
@@ -491,8 +525,28 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="121">
+  <cellXfs count="126">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false" applyFill="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -997,10 +1051,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1042,6 +1096,9 @@
       <c r="I1" s="0" t="s">
         <v>8</v>
       </c>
+      <c r="J1" s="0" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
@@ -1057,19 +1114,22 @@
         <v>1.1</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G2" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="H2" s="1" t="n">
+      <c r="H2" s="2" t="n">
         <v>1.1</v>
       </c>
-      <c r="I2" s="2" t="s">
-        <v>23</v>
+      <c r="I2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1086,18 +1146,21 @@
         <v>2.22</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G3" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="H3" s="3" t="n">
+      <c r="H3" s="5" t="n">
         <v>2.22</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="I3" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="J3" s="4" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1115,19 +1178,22 @@
         <v>3.333</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G4" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="H4" s="5" t="n">
+      <c r="H4" s="8" t="n">
         <v>0.0</v>
       </c>
-      <c r="I4" s="6" t="s">
-        <v>27</v>
+      <c r="I4" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1144,19 +1210,22 @@
         <v>4.4444</v>
       </c>
       <c r="E5" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="0" t="s">
         <v>16</v>
-      </c>
-      <c r="F5" s="0" t="s">
-        <v>15</v>
       </c>
       <c r="G5" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="H5" s="7" t="n">
+      <c r="H5" s="11" t="n">
         <v>0.0</v>
       </c>
-      <c r="I5" s="8" t="s">
-        <v>27</v>
+      <c r="I5" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="J5" s="10" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1166,26 +1235,29 @@
       <c r="B6" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="C6" s="15"/>
+      <c r="C6" s="20"/>
       <c r="D6" s="0" t="n">
         <v>5.5555</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G6" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="H6" s="12"/>
-      <c r="I6" s="16" t="s">
+      <c r="H6" s="17"/>
+      <c r="I6" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="J6" s="13" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="23"/>
+      <c r="A7" s="28"/>
       <c r="B7" s="0" t="n">
         <v>12</v>
       </c>
@@ -1196,26 +1268,27 @@
         <v>6.6666</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="G7" s="20" t="n">
+        <v>14</v>
+      </c>
+      <c r="G7" s="25" t="n">
         <v>30</v>
       </c>
-      <c r="H7" s="24" t="n">
+      <c r="H7" s="29" t="n">
         <v>6.6666</v>
       </c>
-      <c r="I7" s="25" t="s">
-        <v>25</v>
-      </c>
+      <c r="I7" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="J7"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="B8" s="32"/>
+      <c r="B8" s="37"/>
       <c r="C8" s="0" t="n">
         <v>7.7</v>
       </c>
@@ -1223,20 +1296,21 @@
         <v>7.7777</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="G8" s="29" t="s">
-        <v>20</v>
-      </c>
-      <c r="H8" s="33" t="n">
+        <v>12</v>
+      </c>
+      <c r="G8" s="34" t="s">
+        <v>22</v>
+      </c>
+      <c r="H8" s="38" t="n">
         <v>7.7</v>
       </c>
-      <c r="I8" s="34" t="s">
-        <v>23</v>
-      </c>
+      <c r="I8" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="J8"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
@@ -1248,18 +1322,19 @@
       <c r="C9" s="0" t="n">
         <v>8.8</v>
       </c>
-      <c r="D9" s="42"/>
-      <c r="E9" s="45"/>
+      <c r="D9" s="47"/>
+      <c r="E9" s="50"/>
       <c r="F9" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="G9" s="35" t="n">
+        <v>12</v>
+      </c>
+      <c r="G9" s="40" t="n">
         <v>8.0</v>
       </c>
-      <c r="H9" s="39"/>
-      <c r="I9" s="46" t="s">
-        <v>23</v>
-      </c>
+      <c r="H9" s="44"/>
+      <c r="I9" s="51" t="s">
+        <v>26</v>
+      </c>
+      <c r="J9"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
@@ -1274,13 +1349,14 @@
       <c r="D10" s="0" t="n">
         <v>9.9999</v>
       </c>
-      <c r="E10" s="59"/>
-      <c r="F10" s="63" t="s">
-        <v>21</v>
-      </c>
-      <c r="G10" s="49"/>
-      <c r="H10" s="53"/>
-      <c r="I10" s="60"/>
+      <c r="E10" s="64"/>
+      <c r="F10" s="68" t="s">
+        <v>23</v>
+      </c>
+      <c r="G10" s="54"/>
+      <c r="H10" s="58"/>
+      <c r="I10" s="65"/>
+      <c r="J10"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
@@ -1295,24 +1371,26 @@
       <c r="D11" s="0" t="n">
         <v>10.101</v>
       </c>
-      <c r="E11" s="77"/>
-      <c r="F11" s="81"/>
-      <c r="G11" s="67"/>
-      <c r="H11" s="71"/>
-      <c r="I11" s="78"/>
+      <c r="E11" s="82"/>
+      <c r="F11" s="86"/>
+      <c r="G11" s="72"/>
+      <c r="H11" s="76"/>
+      <c r="I11" s="83"/>
+      <c r="J11"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="94"/>
-      <c r="B12" s="97"/>
-      <c r="C12" s="116"/>
-      <c r="D12" s="110"/>
+      <c r="A12" s="99"/>
+      <c r="B12" s="102"/>
+      <c r="C12" s="121"/>
+      <c r="D12" s="115"/>
       <c r="E12" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="F12" s="120"/>
-      <c r="G12" s="91"/>
-      <c r="H12" s="107"/>
-      <c r="I12" s="117"/>
+        <v>24</v>
+      </c>
+      <c r="F12" s="125"/>
+      <c r="G12" s="96"/>
+      <c r="H12" s="112"/>
+      <c r="I12" s="122"/>
+      <c r="J12"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>